<commit_message>
Conclusão final de criação das folhas de pontos e ajustes necessarios.
</commit_message>
<xml_diff>
--- a/funcionarios_sede.xlsx
+++ b/funcionarios_sede.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAC\Desktop\Plano folha de Ponto\ControlePonto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2870AD3-628F-4139-8C98-5D9031368434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87355800-CF38-44BD-BEBB-88C564C38349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VIGIAS" sheetId="1" r:id="rId1"/>
@@ -746,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -810,7 +810,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1195,25 +1198,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="38.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="2" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="38.44140625" style="1"/>
+    <col min="4" max="4" width="34.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="38.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>0.98958333333333304</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>0.29166666666666702</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1416,7 +1419,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>13</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
         <v>14</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
         <v>15</v>
       </c>
@@ -1691,17 +1694,17 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="41.109375" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" customWidth="1"/>
-    <col min="9" max="9" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>1</v>
       </c>
@@ -1727,7 +1730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>3091</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>10777</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -1789,7 +1792,7 @@
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24" s="26"/>
     </row>
   </sheetData>
@@ -1801,24 +1804,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:N81"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.44140625" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1847,18 +1850,18 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="8">
-        <v>12453</v>
+        <v>12158</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>40</v>
@@ -1874,72 +1877,72 @@
       </c>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
-        <v>12821</v>
+        <v>12899</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G3" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="13">
-        <v>0.67708333333333304</v>
+        <v>141</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
-        <v>12517</v>
+        <v>13448</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>30</v>
+        <v>143</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G4" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0.67708333333333304</v>
+        <v>144</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>146</v>
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
-        <v>12899</v>
+        <v>13800</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>43</v>
+        <v>153</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>40</v>
@@ -1947,80 +1950,72 @@
       <c r="G5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
-        <v>13177</v>
+        <v>13799</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>33</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>12164</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="8">
-        <v>13011</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0.67708333333333304</v>
-      </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="20">
-        <v>12156</v>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>12452</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>40</v>
@@ -2036,18 +2031,18 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
-        <v>12158</v>
+        <v>12453</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>40</v>
@@ -2063,18 +2058,18 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
-        <v>12166</v>
+        <v>12498</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>177</v>
+        <v>38</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>40</v>
@@ -2090,18 +2085,18 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
-        <v>12454</v>
+        <v>13128</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>40</v>
@@ -2117,18 +2112,18 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
-        <v>12157</v>
+        <v>12159</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>119</v>
+        <v>53</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>40</v>
@@ -2144,175 +2139,179 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
-        <v>13811</v>
+        <v>12454</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>173</v>
+        <v>54</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="H13" s="10" t="s">
         <v>41</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
-        <v>12886</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="11" t="s">
+        <v>12895</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="21">
+        <v>13824</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>12500</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="13">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>12512</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F17" s="13">
         <v>0.29166666666666702</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G17" s="13">
         <v>0.45833333333333298</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H17" s="13">
         <v>0.5</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I17" s="13">
         <v>0.67708333333333304</v>
       </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="8">
-        <v>12160</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="13">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>12515</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H18" s="13">
         <v>0.5</v>
       </c>
-      <c r="I15" s="13">
-        <v>0.67708333333333337</v>
-      </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="8">
-        <v>12164</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="8">
-        <v>13478</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="8">
-        <v>12163</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>42</v>
+      <c r="I18" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
-        <v>12500</v>
+        <v>12517</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="9" t="s">
         <v>58</v>
       </c>
       <c r="F19" s="13">
@@ -2329,234 +2328,234 @@
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
-        <v>13735</v>
+        <v>12518</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>179</v>
+        <v>62</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="F20" s="13">
-        <v>0.29166666666666669</v>
+        <v>0.29166666666666702</v>
       </c>
       <c r="G20" s="13">
-        <v>0.45833333333333331</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="H20" s="13">
         <v>0.5</v>
       </c>
       <c r="I20" s="13">
-        <v>0.67708333333333337</v>
+        <v>0.67708333333333304</v>
       </c>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
-        <v>12153</v>
+        <v>12519</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>86</v>
+        <v>63</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
-        <v>13849</v>
+        <v>12520</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>80</v>
+        <v>126</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>42</v>
+        <v>58</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H22" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
-        <v>13824</v>
+        <v>12820</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>52</v>
+        <v>127</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
-        <v>12250</v>
+        <v>12821</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>167</v>
+        <v>64</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>42</v>
+        <v>128</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H24" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
-        <v>12165</v>
+        <v>12824</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>104</v>
+        <v>129</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="F25" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="8">
-        <v>13312</v>
+        <v>12883</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>109</v>
+        <v>65</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>42</v>
+        <v>124</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H26" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="8">
-        <v>12894</v>
+        <v>12884</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>181</v>
+        <v>130</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>42</v>
+        <v>168</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
-        <v>12512</v>
+        <v>12885</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F28" s="13">
         <v>0.29166666666666702</v>
@@ -2572,12 +2571,12 @@
       </c>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
-        <v>12883</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>65</v>
+        <v>12886</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>30</v>
@@ -2599,41 +2598,45 @@
       </c>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
-        <v>13081</v>
+        <v>12926</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>84</v>
+        <v>39</v>
+      </c>
+      <c r="F30" s="13">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G30" s="13">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H30" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I30" s="13">
+        <v>0.67708333333333337</v>
       </c>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
-        <v>13390</v>
+        <v>12938</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="F31" s="13">
         <v>0.29166666666666702</v>
@@ -2649,445 +2652,453 @@
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="8">
-        <v>12452</v>
+        <v>13003</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>47</v>
+        <v>69</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="F32" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G32" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H32" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I32" s="13">
+        <v>0.67708333333333304</v>
       </c>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="8">
-        <v>13536</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>151</v>
+        <v>12469</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="F33" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G33" s="13">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="H33" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I33" s="13">
-        <v>0.67708333333333337</v>
+        <v>92</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="8">
-        <v>12926</v>
+        <v>13004</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>177</v>
+        <v>133</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
       <c r="F34" s="13">
-        <v>0.29166666666666669</v>
+        <v>0.29166666666666702</v>
       </c>
       <c r="G34" s="13">
-        <v>0.45833333333333331</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="H34" s="13">
         <v>0.5</v>
       </c>
       <c r="I34" s="13">
-        <v>0.67708333333333337</v>
+        <v>0.67708333333333304</v>
       </c>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="8">
-        <v>13843</v>
+        <v>13010</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="F35" s="13">
-        <v>0.29166666666666669</v>
+        <v>0.29166666666666702</v>
       </c>
       <c r="G35" s="13">
-        <v>0.45833333333333331</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="H35" s="13">
         <v>0.5</v>
       </c>
       <c r="I35" s="13">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="8">
+        <v>13011</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G36" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H36" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I36" s="13">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="8">
+        <v>13041</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G37" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H37" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I37" s="13">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="8">
+        <v>13254</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G38" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H38" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I38" s="13">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="8">
+        <v>13390</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G39" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H39" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I39" s="13">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="8">
+        <v>13391</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="13">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="G40" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="H40" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I40" s="13">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="8">
+        <v>13454</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F41" s="13">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G41" s="13">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H41" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I41" s="13">
         <v>0.67708333333333337</v>
       </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="8">
-        <v>13903</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="8">
-        <v>12140</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="8">
-        <v>12495</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="8">
-        <v>12510</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="8">
-        <v>12895</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="8">
-        <v>13799</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="8">
-        <v>13809</v>
+        <v>13536</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>160</v>
+        <v>151</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>77</v>
+        <v>152</v>
+      </c>
+      <c r="F42" s="13">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G42" s="13">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H42" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I42" s="13">
+        <v>0.67708333333333337</v>
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="8">
-        <v>12159</v>
+        <v>13735</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>52</v>
+        <v>179</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G43" s="13">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H43" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I43" s="13">
+        <v>0.67708333333333337</v>
       </c>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="8">
-        <v>12938</v>
+        <v>13843</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="F44" s="13">
-        <v>0.29166666666666702</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="G44" s="13">
-        <v>0.45833333333333298</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="H44" s="13">
         <v>0.5</v>
       </c>
       <c r="I44" s="13">
-        <v>0.67708333333333304</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="8">
-        <v>13041</v>
+        <v>13833</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="F45" s="13">
-        <v>0.29166666666666702</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="G45" s="13">
-        <v>0.45833333333333298</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="H45" s="13">
         <v>0.5</v>
       </c>
       <c r="I45" s="13">
-        <v>0.67708333333333304</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="8">
-        <v>12519</v>
+        <v>12160</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>30</v>
+        <v>72</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G46" s="13">
-        <v>0.45833333333333298</v>
+        <v>44</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="H46" s="13">
         <v>0.5</v>
       </c>
       <c r="I46" s="13">
-        <v>0.67708333333333304</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="8">
-        <v>13820</v>
+        <v>12166</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>178</v>
+        <v>73</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="8">
-        <v>12880</v>
+        <v>12894</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>75</v>
+        <v>181</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>33</v>
@@ -3100,75 +3111,75 @@
       </c>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="8">
-        <v>13448</v>
+        <v>13903</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>33</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>146</v>
+        <v>42</v>
       </c>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="8">
-        <v>12884</v>
+        <v>12893</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>30</v>
+        <v>78</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="F50" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G50" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H50" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I50" s="13">
-        <v>0.67708333333333304</v>
+        <v>39</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="8">
-        <v>13128</v>
+        <v>12880</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>39</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>33</v>
@@ -3181,18 +3192,18 @@
       </c>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="8">
-        <v>12493</v>
+        <v>13849</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>109</v>
+        <v>186</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>40</v>
@@ -3208,72 +3219,68 @@
       </c>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="8">
-        <v>12893</v>
+        <v>13081</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>75</v>
+        <v>82</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>33</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
       <c r="H53" s="10" t="s">
         <v>41</v>
       </c>
       <c r="I53" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="8">
+        <v>13478</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I54" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J53" s="5"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="8">
-        <v>13003</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F54" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G54" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H54" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I54" s="13">
-        <v>0.67708333333333304</v>
-      </c>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="8">
-        <v>12939</v>
+        <v>12153</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>40</v>
@@ -3289,66 +3296,66 @@
       </c>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="8">
-        <v>12820</v>
+        <v>12163</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>30</v>
+        <v>88</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F56" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G56" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H56" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I56" s="13">
-        <v>0.67708333333333304</v>
+        <v>180</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="8">
-        <v>13810</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>172</v>
+        <v>12483</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>91</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>175</v>
+        <v>42</v>
       </c>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="8">
-        <v>12483</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>95</v>
+        <v>12495</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>91</v>
@@ -3370,72 +3377,72 @@
       </c>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" s="8">
-        <v>12824</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>30</v>
+        <v>12898</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F59" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G59" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H59" s="13">
+        <v>97</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="8">
+        <v>12929</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F60" s="13">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G60" s="13">
         <v>0.5</v>
       </c>
-      <c r="I59" s="13">
-        <v>0.67708333333333304</v>
-      </c>
-      <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B60" s="8">
-        <v>13454</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F60" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G60" s="13">
-        <v>0.45833333333333331</v>
-      </c>
       <c r="H60" s="13">
-        <v>0.5</v>
+        <v>0.51041666666666696</v>
       </c>
       <c r="I60" s="13">
-        <v>0.67708333333333337</v>
+        <v>0.59375</v>
       </c>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="8">
-        <v>11810</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>109</v>
+        <v>13177</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>40</v>
@@ -3451,234 +3458,230 @@
       </c>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="8">
-        <v>12450</v>
+        <v>13497</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" s="8">
-        <v>12929</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>99</v>
+        <v>13810</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>91</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F63" s="13">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G63" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="H63" s="13">
-        <v>0.51041666666666696</v>
-      </c>
-      <c r="I63" s="13">
-        <v>0.59375</v>
+        <v>161</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" s="8">
-        <v>13497</v>
+        <v>13811</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>91</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="F64" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="8">
+        <v>13820</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F65" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G64" s="10" t="s">
+      <c r="G65" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H64" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I64" s="10" t="s">
+      <c r="H65" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I65" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B65" s="8">
-        <v>12515</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F65" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G65" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H65" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I65" s="13">
-        <v>0.67708333333333304</v>
-      </c>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" s="8">
-        <v>12898</v>
+        <v>12140</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="8">
-        <v>13833</v>
+        <v>12165</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>30</v>
+        <v>105</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="F67" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G67" s="13">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="H67" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I67" s="13">
-        <v>0.67708333333333337</v>
+        <v>44</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" s="8">
-        <v>12518</v>
+        <v>12450</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>30</v>
+        <v>106</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F68" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G68" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H68" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I68" s="13">
-        <v>0.67708333333333304</v>
+        <v>44</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H68" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" s="8">
-        <v>12469</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>30</v>
+        <v>12455</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H69" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" s="8">
-        <v>12498</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>49</v>
+        <v>13812</v>
+      </c>
+      <c r="C70" s="28" t="s">
+        <v>163</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>40</v>
@@ -3686,215 +3689,207 @@
       <c r="G70" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H70" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I70" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" s="8">
-        <v>12455</v>
+        <v>13809</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>104</v>
+        <v>160</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>33</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
       <c r="H71" s="10" t="s">
         <v>41</v>
       </c>
       <c r="I71" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="27">
+        <v>11810</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I72" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B72" s="27">
-        <v>13391</v>
-      </c>
-      <c r="C72" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F72" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G72" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H72" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I72" s="13">
-        <v>0.67708333333333304</v>
-      </c>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" s="8">
-        <v>12885</v>
+        <v>12493</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>30</v>
+        <v>110</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F73" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G73" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H73" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I73" s="13">
-        <v>0.67708333333333304</v>
+        <v>44</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" s="8">
-        <v>13004</v>
+        <v>12510</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>30</v>
+        <v>111</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F74" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G74" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H74" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I74" s="13">
-        <v>0.67708333333333304</v>
+        <v>92</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" s="8">
-        <v>13254</v>
+        <v>13312</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>30</v>
+        <v>112</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F75" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G75" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H75" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I75" s="13">
-        <v>0.67708333333333304</v>
+        <v>39</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" s="8">
-        <v>12520</v>
+        <v>12250</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>30</v>
+        <v>166</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F76" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G76" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H76" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I76" s="13">
-        <v>0.67708333333333304</v>
+        <v>92</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I76" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B77" s="8">
-        <v>13010</v>
+        <v>12939</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>30</v>
+        <v>113</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F77" s="13">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G77" s="13">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="H77" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="I77" s="13">
-        <v>0.67708333333333304</v>
+        <v>39</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B78" s="8">
-        <v>13812</v>
-      </c>
-      <c r="C78" s="28" t="s">
-        <v>163</v>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="20">
+        <v>12156</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="F78" s="10" t="s">
         <v>40</v>
@@ -3902,22 +3897,26 @@
       <c r="G78" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H78" s="10"/>
-      <c r="I78" s="10"/>
+      <c r="H78" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" s="8">
-        <v>13800</v>
+        <v>12157</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>40</v>
@@ -3925,10 +3924,14 @@
       <c r="G79" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H79" s="10"/>
-      <c r="I79" s="10"/>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H79" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
@@ -3938,7 +3941,7 @@
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
@@ -3949,9 +3952,6 @@
       <c r="I81" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I79">
-    <sortCondition ref="C2:C79"/>
-  </sortState>
   <pageMargins left="0.19685039370078741" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>